<commit_message>
Started converting spreadsheets to XML
</commit_message>
<xml_diff>
--- a/data/board_data.xlsx
+++ b/data/board_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kingsley\Desktop\SWE2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\users\matthew\projects\github\meme-team-se\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14580" windowHeight="8370" xr2:uid="{3AB37EF7-9957-4EAE-A376-EF9CBBC9245A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14580" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
   </numFmts>
@@ -674,11 +674,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194933F7-920A-45E1-89BC-1AB0AFB7405E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +767,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -820,7 +820,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -876,7 +876,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -897,7 +897,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -958,7 +958,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>34</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>36</v>
       </c>
@@ -1827,7 +1827,7 @@
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>37</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Added the updated board data
</commit_message>
<xml_diff>
--- a/data/board_data.xlsx
+++ b/data/board_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\users\matthew\projects\github\meme-team-se\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Desktop\SWE2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14580" windowHeight="8370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14580" windowHeight="8370" xr2:uid="{3AB37EF7-9957-4EAE-A376-EF9CBBC9245A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="91">
   <si>
     <t>Go</t>
   </si>
@@ -287,19 +287,22 @@
     <t>£150 + 4 houses</t>
   </si>
   <si>
-    <t>Green, Purple</t>
-  </si>
-  <si>
     <t>£200 + 4 houses</t>
   </si>
   <si>
     <t>Income Tax and Super Tax fines are paid to the bank</t>
+  </si>
+  <si>
+    <t>Deep blue</t>
+  </si>
+  <si>
+    <t>Green, Deep blue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
   </numFmts>
@@ -674,11 +677,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194933F7-920A-45E1-89BC-1AB0AFB7405E}">
   <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +770,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -804,6 +807,9 @@
       <c r="H6">
         <v>60</v>
       </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
       <c r="K6">
         <v>10</v>
       </c>
@@ -820,7 +826,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -876,7 +882,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -897,7 +903,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -958,7 +964,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1049,7 +1055,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1102,7 +1108,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1198,7 +1204,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1406,7 +1412,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -1497,7 +1503,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
@@ -1593,7 +1599,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
@@ -1654,7 +1660,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
@@ -1745,7 +1751,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>34</v>
       </c>
@@ -1801,7 +1807,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>36</v>
       </c>
@@ -1827,7 +1833,7 @@
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
     </row>
-    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>37</v>
       </c>
@@ -1856,7 +1862,7 @@
         <v>61</v>
       </c>
       <c r="D42" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="F42" t="s">
         <v>18</v>
@@ -1883,7 +1889,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>39</v>
       </c>
@@ -1912,7 +1918,7 @@
         <v>64</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="F44" t="s">
         <v>18</v>
@@ -2012,13 +2018,13 @@
         <v>75</v>
       </c>
       <c r="H51" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="J51" s="5">
         <v>200</v>
       </c>
       <c r="K51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2028,7 +2034,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>